<commit_message>
factor(test): adapt TestOneTabCreatedController tests
</commit_message>
<xml_diff>
--- a/fichiers_xls/testongletbyparticipant-result.xlsx
+++ b/fichiers_xls/testongletbyparticipant-result.xlsx
@@ -8,8 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="test" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Feuille2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="test" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Feuille2" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t xml:space="preserve">user</t>
   </si>
@@ -54,6 +54,42 @@
   </si>
   <si>
     <t xml:space="preserve">Identifiers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22300896</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4479</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8814</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6286</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15306</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22303499</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11301</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22302237</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4574</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7308</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4518</t>
   </si>
 </sst>
 </file>
@@ -134,11 +170,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -237,8 +273,114 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1284,63 +1426,63 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>22300896</v>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>4479</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>8814</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>6286</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>15306</v>
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>22303499</v>
-      </c>
-      <c r="B3" s="2" t="n">
-        <v>9003</v>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>11301</v>
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>22302237</v>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>4574</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>7308</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>4518</v>
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>